<commit_message>
Finalizado os testes de equivalência
</commit_message>
<xml_diff>
--- a/teste equivalencia/classes_de_equivalencia.xlsx
+++ b/teste equivalencia/classes_de_equivalencia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20222014040015\Desktop\teste_software\teste-de-software\teste equivalencia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\OneDrive\Documentos\IFRN\período 5\Testes\teste-de-software\teste equivalencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B9B23-3F7C-4127-AB47-39EF32843884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Rolteiro de teste: Verificar se é triângulo</t>
   </si>
@@ -105,12 +106,15 @@
   </si>
   <si>
     <t>Valores negativos e 0</t>
+  </si>
+  <si>
+    <t>A != B e B != C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,6 +296,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -300,18 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,12 +329,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -606,11 +610,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,28 +626,28 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -651,8 +655,8 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -660,8 +664,8 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -669,8 +673,8 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -679,28 +683,28 @@
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -708,8 +712,8 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -717,43 +721,43 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -761,92 +765,87 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
     <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
     </row>
     <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="8"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="3" t="s">
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="12"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -854,7 +853,7 @@
   <mergeCells count="8">
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B29:B33"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B11:D11"/>

</xml_diff>

<commit_message>
Criando valor limite para modelo do triangulo
</commit_message>
<xml_diff>
--- a/teste equivalencia/classes_de_equivalencia.xlsx
+++ b/teste equivalencia/classes_de_equivalencia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\OneDrive\Documentos\IFRN\período 5\Testes\teste-de-software\teste equivalencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B9B23-3F7C-4127-AB47-39EF32843884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B081D3B-2814-47BA-A577-9EA20449C631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Rolteiro de teste: Verificar se é triângulo</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>A != B e B != C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limite inferior </t>
+  </si>
+  <si>
+    <t>Limite superior</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -280,11 +286,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,6 +355,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -611,28 +646,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="20.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -642,8 +677,14 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
@@ -653,8 +694,12 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -662,8 +707,12 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="11"/>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -671,8 +720,12 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -680,16 +733,20 @@
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
@@ -699,8 +756,14 @@
       <c r="D12" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
@@ -710,8 +773,12 @@
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="5" t="s">
         <v>14</v>
@@ -719,30 +786,42 @@
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="5"/>
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>1</v>
       </c>
@@ -752,8 +831,14 @@
       <c r="D20" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>4</v>
       </c>
@@ -763,8 +848,12 @@
       <c r="D21" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="5" t="s">
         <v>21</v>
@@ -772,8 +861,12 @@
       <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="5" t="s">
         <v>22</v>
@@ -781,23 +874,31 @@
       <c r="D23" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="3"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
@@ -807,8 +908,14 @@
       <c r="D28" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>4</v>
       </c>
@@ -818,8 +925,12 @@
       <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="5" t="s">
         <v>14</v>
@@ -827,38 +938,50 @@
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="5"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="6"/>
       <c r="D33" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>